<commit_message>
Front para importar tarbela de itens, pronto
</commit_message>
<xml_diff>
--- a/relatorios/relatorio_quantidade_itens.xlsx
+++ b/relatorios/relatorio_quantidade_itens.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -433,11 +433,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="30" customWidth="1" min="2" max="2"/>
-    <col width="40" customWidth="1" min="3" max="3"/>
-    <col width="15" customWidth="1" min="4" max="4"/>
-    <col width="20" customWidth="1" min="5" max="5"/>
+    <col width="14" customWidth="1" min="1" max="1"/>
+    <col width="21" customWidth="1" min="2" max="2"/>
+    <col width="25" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="15" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -469,20 +469,20 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>INFORMATICA</t>
+          <t>LIMPEZA</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Teste</t>
+          <t>Sabaoembarra</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E2" t="inlineStr"/>
     </row>
@@ -497,51 +497,443 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Tecladousb</t>
+          <t>Cabousb</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>INFORMATICA</t>
+          <t>PAPELARIA</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Mouseusb</t>
+          <t>Lapis</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
+        <v>22</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>MATERIAISSALADEAULA</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Apagador</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
         <v>24</v>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B6" t="inlineStr">
         <is>
           <t>INFORMATICA</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Teste</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>5</v>
+      </c>
+      <c r="E6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>27</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>FERRAMENTAS</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Chavedefenda</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>20</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>PAPELARIA</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Cadernoespiral</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>50</v>
+      </c>
+      <c r="E8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>20</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>PAPELARIA</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Borrachabranca</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>20</v>
+      </c>
+      <c r="E9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>26</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>LIMPEZA</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Detergente</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>26</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>LIMPEZA</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Sabaoliquido</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>200</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>26</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>LIMPEZA</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Cadernoespiral</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>100</v>
+      </c>
+      <c r="E12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>26</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>LIMPEZA</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Papela1Sulfite</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>10</v>
+      </c>
+      <c r="E13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>26</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>LIMPEZA</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Borrachabranca</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>40</v>
+      </c>
+      <c r="E14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>20</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>PAPELARIA</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Canetaesferograficaazul</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>300</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>24</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>INFORMATICA</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Mouseusb</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>28</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>MATERIALESCOLAR</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Cadernoespiral</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>100</v>
+      </c>
+      <c r="E17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>24</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>INFORMATICA</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
         <is>
           <t>Cabovga</t>
         </is>
       </c>
-      <c r="D5" t="n">
+      <c r="D18" t="n">
+        <v>1</v>
+      </c>
+      <c r="E18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>20</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>PAPELARIA</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Papela4Sulfite</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>15</v>
+      </c>
+      <c r="E19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>28</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>MATERIALESCOLAR</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Borrachabranca</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>40</v>
+      </c>
+      <c r="E20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>PAPELARIA</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Canetapreta</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
         <v>4</v>
       </c>
-      <c r="E5" t="inlineStr"/>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>10/12/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>PAPELARIA</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Canetaazul</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>4</v>
+      </c>
+      <c r="E22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>26</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>LIMPEZA</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Sabaoempo</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>2</v>
+      </c>
+      <c r="E23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>24</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>INFORMATICA</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Tecladousb</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>20</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>PAPELARIA</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Canetavermelha</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>100</v>
+      </c>
+      <c r="E25" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Correção nos códigos de geração de relatórios
</commit_message>
<xml_diff>
--- a/relatorios/relatorio_quantidade_itens.xlsx
+++ b/relatorios/relatorio_quantidade_itens.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -435,7 +435,7 @@
   <cols>
     <col width="14" customWidth="1" min="1" max="1"/>
     <col width="17" customWidth="1" min="2" max="2"/>
-    <col width="25" customWidth="1" min="3" max="3"/>
+    <col width="27" customWidth="1" min="3" max="3"/>
     <col width="12" customWidth="1" min="4" max="4"/>
     <col width="15" customWidth="1" min="5" max="5"/>
   </cols>
@@ -478,34 +478,30 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Sabaoliquido</t>
+          <t>Sabão Em Barra</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>600</v>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>31/12/2025</t>
-        </is>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>LIMPEZA</t>
+          <t>PAPELARIA</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Sabaoembarra</t>
+          <t>Borracha Branca</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" t="inlineStr"/>
     </row>
@@ -520,7 +516,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Chavedefenda</t>
+          <t>Chave De Fenda</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -530,54 +526,54 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>PAPELARIA</t>
+          <t>MATERIALESCOLAR</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Borrachabranca</t>
+          <t>Caderno Espiral</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>20</v>
+        <v>200</v>
       </c>
       <c r="E5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>LIMPEZA</t>
+          <t>PAPELARIA</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Papela1Sulfite</t>
+          <t>Papel A4 Sulfite</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>LIMPEZA</t>
+          <t>INFORMATICA</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Detergente</t>
+          <t>Mouse Usb</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -587,24 +583,24 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>DIVERSOS</t>
+          <t>PAPELARIA</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Garrafadeagua</t>
+          <t>Caneta Preta</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>11/06/2025</t>
+          <t>10/12/2025</t>
         </is>
       </c>
     </row>
@@ -619,139 +615,131 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Canetaesferograficaazul</t>
+          <t>Caneta Azul</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>300</v>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>31/12/2025</t>
-        </is>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="E9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>INFORMATICA</t>
+          <t>LIMPEZA</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Mouseusb</t>
+          <t>Sabão Em Pó</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>MATERIALESCOLAR</t>
+          <t>PAPELARIA</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Cadernoespiral</t>
+          <t>Lápis</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="E11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>INFORMATICA</t>
+          <t>ELETRICOS</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Cabovga</t>
+          <t>Filtro De Linha</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="E12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>PAPELARIA</t>
+          <t>LIMPEZA</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Papela4Sulfite</t>
+          <t>Sabão Líquido</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>15</v>
-      </c>
-      <c r="E13" t="inlineStr"/>
+        <v>800</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
+        <v>26</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>LIMPEZA</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Papel A1 Sulfite</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
         <v>29</v>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>DIVERSOS</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Acucar</t>
-        </is>
-      </c>
-      <c r="D14" t="n">
-        <v>50</v>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>13/06/2025</t>
-        </is>
-      </c>
+      <c r="E14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>PAPELARIA</t>
+          <t>INFORMATICA</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Canetapreta</t>
+          <t>Teclado Usb</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>4</v>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>10/12/2025</t>
-        </is>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="E15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -764,129 +752,103 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Canetaazul</t>
+          <t>Caneta Vermelha</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>4</v>
+        <v>99</v>
       </c>
       <c r="E16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>LIMPEZA</t>
+          <t>DIVERSOS</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Sabaoempo</t>
+          <t>Café</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>2</v>
-      </c>
-      <c r="E17" t="inlineStr"/>
+        <v>20</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>19/06/2025</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>INFORMATICA</t>
+          <t>DIVERSOS</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Tecladousb</t>
+          <t>Açúcar</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>0</v>
-      </c>
-      <c r="E18" t="inlineStr"/>
+        <v>49</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>13/06/2025</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>PAPELARIA</t>
+          <t>DIVERSOS</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Lapis</t>
+          <t>Garrafa De Água</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>4</v>
-      </c>
-      <c r="E19" t="inlineStr"/>
+        <v>19</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>11/06/2025</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>ELETRICOS</t>
+          <t>PAPELARIA</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Filtrodelinha</t>
+          <t>Caneta Esferográfica Azul</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>20</v>
-      </c>
-      <c r="E20" t="inlineStr"/>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>20</v>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>PAPELARIA</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Canetavermelha</t>
-        </is>
-      </c>
-      <c r="D21" t="n">
-        <v>99</v>
-      </c>
-      <c r="E21" t="inlineStr"/>
-    </row>
-    <row r="22">
-      <c r="A22" t="n">
-        <v>29</v>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>DIVERSOS</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>Cafe</t>
-        </is>
-      </c>
-      <c r="D22" t="n">
-        <v>20</v>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>19/06/2025</t>
+        <v>490</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
         </is>
       </c>
     </row>

</xml_diff>